<commit_message>
Update tolerances for correct volume implementation in matlab code
</commit_message>
<xml_diff>
--- a/SBTAB_Fujita_2010.xlsx
+++ b/SBTAB_Fujita_2010.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santos\Documents\Git\Thesis_Code\Subcellular_Workflow_Matlab\Model\Model_Fujita_2010\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5CCB81-291D-4419-9A5F-B1DCB88B43C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B4A604-D2F2-4DBF-A85C-23E2FA1A4E96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21196" tabRatio="857" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="275">
   <si>
     <t>!!SBtab</t>
   </si>
@@ -263,9 +263,6 @@
   </si>
   <si>
     <t>!Value:log2</t>
-  </si>
-  <si>
-    <t>nanomolarity</t>
   </si>
   <si>
     <t>Experiment 1</t>
@@ -538,9 +535,6 @@
     <t>EGF</t>
   </si>
   <si>
-    <t>True</t>
-  </si>
-  <si>
     <t>10.1126/scisignal.2000811</t>
   </si>
   <si>
@@ -775,9 +769,6 @@
     <t>V1</t>
   </si>
   <si>
-    <t>femtoliter</t>
-  </si>
-  <si>
     <t>Document='Fujita_2010' TableName='Compound' TableType='Compound' TableTitle='Fujita_2010 Compounds'</t>
   </si>
   <si>
@@ -903,6 +894,12 @@
   <si>
     <t>SBtabVersion='1.0' Document='Fujita_2010' TableName='Compartment' TableTitle='Fujita_2010 Compound' TableType = 'Quantity'</t>
   </si>
+  <si>
+    <t>liter</t>
+  </si>
+  <si>
+    <t>nanomole/liter</t>
+  </si>
 </sst>
 </file>
 
@@ -1009,7 +1006,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1071,9 +1068,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1465,7 +1459,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1475,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1489,21 +1483,21 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
+        <v>273</v>
+      </c>
+      <c r="D3" s="35">
+        <v>1.0000000000000001E-15</v>
       </c>
     </row>
   </sheetData>
@@ -1534,15 +1528,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -2303,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -2326,10 +2320,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -3327,15 +3321,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -4096,7 +4090,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -4119,10 +4113,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -5120,15 +5114,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -5889,7 +5883,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -5912,10 +5906,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -6913,15 +6907,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -7682,7 +7676,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -7705,10 +7699,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -8706,15 +8700,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -9475,7 +9469,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -9498,10 +9492,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -10484,7 +10478,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:J1"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75"/>
@@ -10508,17 +10502,17 @@
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="O1" s="26"/>
     </row>
     <row r="2" spans="1:27" ht="13.5">
@@ -10538,10 +10532,10 @@
         <v>19</v>
       </c>
       <c r="F2" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="29" t="s">
         <v>73</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>74</v>
       </c>
       <c r="H2" s="26" t="s">
         <v>20</v>
@@ -10559,13 +10553,13 @@
         <v>22</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="26">
-        <v>0</v>
+        <v>274</v>
+      </c>
+      <c r="D3" s="9">
+        <v>68190.2</v>
       </c>
       <c r="E3" s="26" t="b">
         <f>FALSE()</f>
@@ -10583,10 +10577,10 @@
         <v>23</v>
       </c>
       <c r="I3" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="26" t="s">
         <v>91</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>92</v>
       </c>
       <c r="O3" s="26"/>
     </row>
@@ -10595,10 +10589,10 @@
         <v>24</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>63</v>
+        <v>274</v>
       </c>
       <c r="D4" s="26">
         <v>0</v>
@@ -10619,10 +10613,10 @@
         <v>23</v>
       </c>
       <c r="I4" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="26" t="s">
         <v>91</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>92</v>
       </c>
       <c r="O4" s="26"/>
     </row>
@@ -10631,10 +10625,10 @@
         <v>25</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>63</v>
+        <v>274</v>
       </c>
       <c r="D5" s="26">
         <v>0</v>
@@ -10655,10 +10649,10 @@
         <v>23</v>
       </c>
       <c r="I5" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J5" s="26" t="s">
         <v>91</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>92</v>
       </c>
       <c r="O5" s="26"/>
     </row>
@@ -10667,13 +10661,13 @@
         <v>26</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="26">
-        <v>0</v>
+        <v>274</v>
+      </c>
+      <c r="D6" s="9">
+        <v>4.3309E-2</v>
       </c>
       <c r="E6" s="26" t="b">
         <f>FALSE()</f>
@@ -10691,10 +10685,10 @@
         <v>23</v>
       </c>
       <c r="I6" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" s="26" t="s">
         <v>91</v>
-      </c>
-      <c r="J6" s="26" t="s">
-        <v>92</v>
       </c>
       <c r="O6" s="26"/>
     </row>
@@ -10703,10 +10697,10 @@
         <v>27</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>63</v>
+        <v>274</v>
       </c>
       <c r="D7" s="26">
         <v>0</v>
@@ -10727,10 +10721,10 @@
         <v>23</v>
       </c>
       <c r="I7" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="26" t="s">
         <v>91</v>
-      </c>
-      <c r="J7" s="26" t="s">
-        <v>92</v>
       </c>
       <c r="K7" s="32"/>
       <c r="L7" s="32"/>
@@ -10752,16 +10746,16 @@
     </row>
     <row r="8" spans="1:27" ht="14.25">
       <c r="A8" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="26">
-        <v>0</v>
+        <v>274</v>
+      </c>
+      <c r="D8" s="9">
+        <v>3.5431699999999999</v>
       </c>
       <c r="E8" s="26" t="b">
         <f>FALSE()</f>
@@ -10779,22 +10773,22 @@
         <v>23</v>
       </c>
       <c r="I8" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="26" t="s">
         <v>91</v>
-      </c>
-      <c r="J8" s="26" t="s">
-        <v>92</v>
       </c>
       <c r="O8" s="26"/>
     </row>
     <row r="9" spans="1:27" ht="14.25">
       <c r="A9" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="30" t="s">
-        <v>85</v>
-      </c>
       <c r="C9" s="31" t="s">
-        <v>63</v>
+        <v>274</v>
       </c>
       <c r="D9" s="26">
         <v>0</v>
@@ -10815,22 +10809,22 @@
         <v>23</v>
       </c>
       <c r="I9" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="26" t="s">
         <v>91</v>
-      </c>
-      <c r="J9" s="26" t="s">
-        <v>92</v>
       </c>
       <c r="O9" s="26"/>
     </row>
     <row r="10" spans="1:27" ht="14.25">
       <c r="A10" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>63</v>
+        <v>274</v>
       </c>
       <c r="D10" s="26">
         <v>0</v>
@@ -10851,22 +10845,22 @@
         <v>23</v>
       </c>
       <c r="I10" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="26" t="s">
         <v>91</v>
-      </c>
-      <c r="J10" s="26" t="s">
-        <v>92</v>
       </c>
       <c r="O10" s="26"/>
     </row>
     <row r="11" spans="1:27" ht="14.25">
       <c r="A11" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>63</v>
+        <v>274</v>
       </c>
       <c r="D11" s="26">
         <v>0</v>
@@ -10887,31 +10881,33 @@
         <v>23</v>
       </c>
       <c r="I11" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="26" t="s">
         <v>91</v>
-      </c>
-      <c r="J11" s="26" t="s">
-        <v>92</v>
       </c>
       <c r="O11" s="26"/>
     </row>
     <row r="12" spans="1:27" ht="14.25">
       <c r="A12" s="26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>63</v>
+        <v>274</v>
       </c>
       <c r="D12" s="26">
         <v>0</v>
       </c>
-      <c r="E12" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>154</v>
+      <c r="E12" s="33" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="33" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G12" s="26" t="b">
         <f>FALSE()</f>
@@ -10921,31 +10917,33 @@
         <v>23</v>
       </c>
       <c r="I12" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="26" t="s">
         <v>91</v>
-      </c>
-      <c r="J12" s="26" t="s">
-        <v>92</v>
       </c>
       <c r="O12" s="26"/>
     </row>
     <row r="13" spans="1:27" ht="14.25">
       <c r="A13" s="26" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="34">
-        <v>0</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="F13" s="33" t="s">
-        <v>154</v>
+        <v>274</v>
+      </c>
+      <c r="D13" s="9">
+        <v>68190.2</v>
+      </c>
+      <c r="E13" s="33" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="33" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G13" s="26" t="b">
         <f>FALSE()</f>
@@ -10955,10 +10953,10 @@
         <v>23</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="O13" s="26"/>
     </row>
@@ -11640,15 +11638,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -12409,7 +12407,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -12432,10 +12430,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -13433,15 +13431,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -14202,7 +14200,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -14225,10 +14223,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -15226,15 +15224,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -15995,7 +15993,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -16018,10 +16016,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -17019,15 +17017,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -17788,7 +17786,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -17811,10 +17809,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -18812,15 +18810,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -19581,7 +19579,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -19604,10 +19602,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -20612,7 +20610,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="7"/>
@@ -20687,17 +20685,17 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="15" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -20728,17 +20726,17 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D4" s="15" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -20769,17 +20767,17 @@
         <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -20810,17 +20808,17 @@
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -20845,23 +20843,23 @@
     </row>
     <row r="7" spans="1:26" ht="13.5">
       <c r="A7" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" s="15" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -20886,23 +20884,23 @@
     </row>
     <row r="8" spans="1:26" ht="13.5">
       <c r="A8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D8" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -20927,23 +20925,23 @@
     </row>
     <row r="9" spans="1:26" ht="13.5">
       <c r="A9" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -20968,23 +20966,23 @@
     </row>
     <row r="10" spans="1:26" ht="13.5">
       <c r="A10" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D10" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -21009,23 +21007,23 @@
     </row>
     <row r="11" spans="1:26" ht="13.5">
       <c r="A11" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -21050,23 +21048,23 @@
     </row>
     <row r="12" spans="1:26" ht="13.5">
       <c r="A12" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D12" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -21091,23 +21089,23 @@
     </row>
     <row r="13" spans="1:26" ht="13.5">
       <c r="A13" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D13" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -21245,15 +21243,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -22014,7 +22012,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -22037,10 +22035,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -22121,7 +22119,7 @@
       <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="35">
         <v>9.0092383313698996E-5</v>
       </c>
       <c r="H4">
@@ -23038,15 +23036,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -23807,7 +23805,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -23830,10 +23828,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -23914,7 +23912,7 @@
       <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="35">
         <v>2.6076863961724901E-4</v>
       </c>
       <c r="H4">
@@ -24831,15 +24829,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -25600,7 +25598,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -25623,10 +25621,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -25707,7 +25705,7 @@
       <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="35">
         <v>7.74295778326481E-4</v>
       </c>
       <c r="H4">
@@ -26624,15 +26622,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -27393,7 +27391,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -27416,10 +27414,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -27500,7 +27498,7 @@
       <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="35">
         <v>1.7761848137009401E-3</v>
       </c>
       <c r="H4">
@@ -28417,15 +28415,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -29186,7 +29184,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -29209,10 +29207,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -29293,7 +29291,7 @@
       <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="35">
         <v>3.2994828878185698E-3</v>
       </c>
       <c r="H4">
@@ -30195,7 +30193,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -30217,7 +30215,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -30279,10 +30277,10 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E3" s="25">
         <f t="shared" ref="E3:E16" si="0">10^F3</f>
@@ -30292,10 +30290,10 @@
         <v>-2.1714586807558929</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="10"/>
@@ -30310,13 +30308,13 @@
     </row>
     <row r="4" spans="1:19" ht="14.25">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E4" s="25">
         <f t="shared" si="0"/>
@@ -30326,10 +30324,10 @@
         <v>-1.3898830445880721</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="10"/>
@@ -30344,13 +30342,13 @@
     </row>
     <row r="5" spans="1:19" ht="14.25">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E5" s="25">
         <f t="shared" si="0"/>
@@ -30360,10 +30358,10 @@
         <v>-4.8084651529932163</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="10"/>
@@ -30378,13 +30376,13 @@
     </row>
     <row r="6" spans="1:19" ht="14.25">
       <c r="A6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E6" s="25">
         <f t="shared" si="0"/>
@@ -30394,10 +30392,10 @@
         <v>-2.2861123053046994</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="10"/>
@@ -30412,13 +30410,13 @@
     </row>
     <row r="7" spans="1:19" ht="12.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E7" s="25">
         <f t="shared" si="0"/>
@@ -30428,10 +30426,10 @@
         <v>-1.5147272923617776</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="10"/>
@@ -30446,13 +30444,13 @@
     </row>
     <row r="8" spans="1:19" ht="14.25">
       <c r="A8" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E8" s="25">
         <f t="shared" si="0"/>
@@ -30462,10 +30460,10 @@
         <v>-1.0012203432596507</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="10"/>
@@ -30480,13 +30478,13 @@
     </row>
     <row r="9" spans="1:19" ht="14.25">
       <c r="A9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E9" s="25">
         <f t="shared" si="0"/>
@@ -30496,10 +30494,10 @@
         <v>-5.6773900160161705</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="10"/>
@@ -30514,13 +30512,13 @@
     </row>
     <row r="10" spans="1:19" ht="14.25">
       <c r="A10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E10" s="25">
         <f t="shared" si="0"/>
@@ -30530,10 +30528,10 @@
         <v>-14.285720547548516</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="10"/>
@@ -30548,13 +30546,13 @@
     </row>
     <row r="11" spans="1:19" ht="14.25">
       <c r="A11" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E11" s="25">
         <f t="shared" si="0"/>
@@ -30564,10 +30562,10 @@
         <v>-2.9154308710048689</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="10"/>
@@ -30582,13 +30580,13 @@
     </row>
     <row r="12" spans="1:19" ht="14.25">
       <c r="A12" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E12" s="25">
         <f t="shared" si="0"/>
@@ -30598,10 +30596,10 @@
         <v>-1.4841764738077223</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="10"/>
@@ -30616,13 +30614,13 @@
     </row>
     <row r="13" spans="1:19" ht="14.25">
       <c r="A13" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E13" s="25">
         <f>10^F13</f>
@@ -30632,10 +30630,10 @@
         <v>-2.9465297153107599</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="10"/>
@@ -30650,13 +30648,13 @@
     </row>
     <row r="14" spans="1:19" ht="14.25">
       <c r="A14" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E14" s="25">
         <f t="shared" si="0"/>
@@ -30666,10 +30664,10 @@
         <v>-1.7158152480038114</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="10"/>
@@ -30684,13 +30682,13 @@
     </row>
     <row r="15" spans="1:19" ht="14.25">
       <c r="A15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E15" s="25">
         <f t="shared" si="0"/>
@@ -30700,10 +30698,10 @@
         <v>-3.9731155198115515</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="10"/>
@@ -30718,13 +30716,13 @@
     </row>
     <row r="16" spans="1:19" ht="14.25">
       <c r="A16" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E16" s="25">
         <f t="shared" si="0"/>
@@ -30734,10 +30732,10 @@
         <v>-3.9731155198115515</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="10"/>
@@ -30884,15 +30882,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -31653,7 +31651,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -31676,10 +31674,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -31760,7 +31758,7 @@
       <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="35">
         <v>4.4824817429268997E-3</v>
       </c>
       <c r="H4">
@@ -32677,15 +32675,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -33432,7 +33430,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomRight" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75"/>
@@ -33457,7 +33455,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
@@ -33548,10 +33546,10 @@
         <v>34</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D3" s="18" t="str">
         <f>_xlfn.CONCAT("SD_",A3)</f>
@@ -33560,8 +33558,8 @@
       <c r="E3" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>63</v>
+      <c r="F3" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>36</v>
@@ -33571,10 +33569,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="J3" s="35" t="s">
-        <v>196</v>
+        <v>90</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>194</v>
       </c>
       <c r="L3" s="18"/>
       <c r="M3" s="16"/>
@@ -33603,10 +33601,10 @@
         <v>37</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D4" s="18" t="str">
         <f t="shared" ref="D4:D16" si="0">_xlfn.CONCAT("SD_",A4)</f>
@@ -33615,8 +33613,8 @@
       <c r="E4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>63</v>
+      <c r="F4" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>36</v>
@@ -33626,10 +33624,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="J4" s="35" t="s">
-        <v>197</v>
+        <v>90</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>195</v>
       </c>
       <c r="K4" s="17"/>
       <c r="L4" s="18"/>
@@ -33656,13 +33654,13 @@
     </row>
     <row r="5" spans="1:32" ht="14.25">
       <c r="A5" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D5" s="18" t="str">
         <f t="shared" si="0"/>
@@ -33671,8 +33669,8 @@
       <c r="E5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>63</v>
+      <c r="F5" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>36</v>
@@ -33682,10 +33680,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="J5" s="35" t="s">
-        <v>198</v>
+        <v>90</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>196</v>
       </c>
       <c r="K5" s="17"/>
       <c r="L5" s="18"/>
@@ -33712,10 +33710,10 @@
     </row>
     <row r="6" spans="1:32" ht="14.25">
       <c r="A6" s="18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D6" s="18" t="str">
         <f t="shared" si="0"/>
@@ -33724,8 +33722,8 @@
       <c r="E6" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>63</v>
+      <c r="F6" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>36</v>
@@ -33735,10 +33733,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
@@ -33765,10 +33763,10 @@
     </row>
     <row r="7" spans="1:32" ht="14.25">
       <c r="A7" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D7" s="18" t="str">
         <f t="shared" si="0"/>
@@ -33777,8 +33775,8 @@
       <c r="E7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="16" t="s">
-        <v>63</v>
+      <c r="F7" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>36</v>
@@ -33788,10 +33786,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
@@ -33818,10 +33816,10 @@
     </row>
     <row r="8" spans="1:32" ht="14.25">
       <c r="A8" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D8" s="18" t="str">
         <f t="shared" si="0"/>
@@ -33830,8 +33828,8 @@
       <c r="E8" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>63</v>
+      <c r="F8" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>36</v>
@@ -33841,10 +33839,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
@@ -33871,10 +33869,10 @@
     </row>
     <row r="9" spans="1:32" ht="14.25">
       <c r="A9" s="18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="18" t="str">
@@ -33884,8 +33882,8 @@
       <c r="E9" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>63</v>
+      <c r="F9" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>36</v>
@@ -33895,10 +33893,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
@@ -33925,10 +33923,10 @@
     </row>
     <row r="10" spans="1:32" ht="14.25">
       <c r="A10" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="18" t="str">
@@ -33938,8 +33936,8 @@
       <c r="E10" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>63</v>
+      <c r="F10" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>36</v>
@@ -33949,10 +33947,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
@@ -33979,10 +33977,10 @@
     </row>
     <row r="11" spans="1:32" ht="14.25">
       <c r="A11" s="18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="str">
@@ -33992,8 +33990,8 @@
       <c r="E11" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="16" t="s">
-        <v>63</v>
+      <c r="F11" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>36</v>
@@ -34003,10 +34001,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
@@ -34033,10 +34031,10 @@
     </row>
     <row r="12" spans="1:32" ht="14.25">
       <c r="A12" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="18" t="str">
@@ -34046,8 +34044,8 @@
       <c r="E12" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>63</v>
+      <c r="F12" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>36</v>
@@ -34057,10 +34055,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
@@ -34087,10 +34085,10 @@
     </row>
     <row r="13" spans="1:32" ht="14.25">
       <c r="A13" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="18" t="str">
@@ -34100,8 +34098,8 @@
       <c r="E13" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>63</v>
+      <c r="F13" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>36</v>
@@ -34111,10 +34109,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
@@ -34141,10 +34139,10 @@
     </row>
     <row r="14" spans="1:32" ht="14.25">
       <c r="A14" s="18" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="18" t="str">
@@ -34154,8 +34152,8 @@
       <c r="E14" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>63</v>
+      <c r="F14" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G14" s="16" t="s">
         <v>36</v>
@@ -34165,10 +34163,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
@@ -34195,10 +34193,10 @@
     </row>
     <row r="15" spans="1:32" ht="14.25">
       <c r="A15" s="18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="18" t="str">
@@ -34208,8 +34206,8 @@
       <c r="E15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="16" t="s">
-        <v>63</v>
+      <c r="F15" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>36</v>
@@ -34219,10 +34217,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
@@ -34249,10 +34247,10 @@
     </row>
     <row r="16" spans="1:32" ht="14.25">
       <c r="A16" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="18" t="str">
@@ -34262,8 +34260,8 @@
       <c r="E16" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="16" t="s">
-        <v>63</v>
+      <c r="F16" s="31" t="s">
+        <v>274</v>
       </c>
       <c r="G16" s="16" t="s">
         <v>36</v>
@@ -34273,10 +34271,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J16" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
@@ -34384,13 +34382,13 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O3" sqref="O3:O20"/>
+      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="6.73046875" style="20"/>
-    <col min="2" max="2" width="129.73046875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.265625" style="20" customWidth="1"/>
     <col min="3" max="3" width="11.59765625" style="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.265625" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.3984375" style="20" bestFit="1" customWidth="1"/>
@@ -34412,7 +34410,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
@@ -34459,19 +34457,19 @@
         <v>41</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="I2" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="J2" s="17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>21</v>
@@ -34502,14 +34500,14 @@
         <v>38</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>45</v>
@@ -34530,7 +34528,7 @@
         <v>68190.2</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M3" s="18">
         <v>-120</v>
@@ -34556,17 +34554,17 @@
     </row>
     <row r="4" spans="1:26" ht="14.25">
       <c r="A4" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>75</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>76</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>45</v>
@@ -34587,7 +34585,7 @@
         <v>68190.2</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M4" s="18">
         <v>-120</v>
@@ -34613,17 +34611,17 @@
     </row>
     <row r="5" spans="1:26" ht="14.25">
       <c r="A5" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>78</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>45</v>
@@ -34644,7 +34642,7 @@
         <v>68190.2</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M5" s="18">
         <v>-120</v>
@@ -34670,17 +34668,17 @@
     </row>
     <row r="6" spans="1:26" ht="14.25">
       <c r="A6" s="18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>45</v>
@@ -34701,7 +34699,7 @@
         <v>68190.2</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M6" s="18">
         <v>-120</v>
@@ -34727,17 +34725,17 @@
     </row>
     <row r="7" spans="1:26" ht="14.25">
       <c r="A7" s="18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>45</v>
@@ -34758,7 +34756,7 @@
         <v>68190.2</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M7" s="18">
         <v>-120</v>
@@ -34784,17 +34782,17 @@
     </row>
     <row r="8" spans="1:26" ht="14.25">
       <c r="A8" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F8" s="18" t="s">
         <v>45</v>
@@ -34815,7 +34813,7 @@
         <v>68190.2</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M8" s="18">
         <v>-120</v>
@@ -34841,17 +34839,17 @@
     </row>
     <row r="9" spans="1:26" ht="14.25">
       <c r="A9" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>45</v>
@@ -34872,7 +34870,7 @@
         <v>68190.2</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M9" s="18">
         <v>-120</v>
@@ -34898,17 +34896,17 @@
     </row>
     <row r="10" spans="1:26" ht="14.25">
       <c r="A10" s="18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>45</v>
@@ -34929,7 +34927,7 @@
         <v>68190.2</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M10" s="18">
         <v>-120</v>
@@ -34955,17 +34953,17 @@
     </row>
     <row r="11" spans="1:26" ht="14.25">
       <c r="A11" s="18" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>45</v>
@@ -34986,7 +34984,7 @@
         <v>68190.2</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M11" s="18">
         <v>-120</v>
@@ -35012,17 +35010,17 @@
     </row>
     <row r="12" spans="1:26" ht="14.25">
       <c r="A12" s="18" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>45</v>
@@ -35043,7 +35041,7 @@
         <v>68190.2</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M12" s="18">
         <v>-120</v>
@@ -35069,17 +35067,17 @@
     </row>
     <row r="13" spans="1:26" ht="14.25">
       <c r="A13" s="18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>45</v>
@@ -35100,7 +35098,7 @@
         <v>68190.2</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M13" s="18">
         <v>-120</v>
@@ -35126,17 +35124,17 @@
     </row>
     <row r="14" spans="1:26" ht="14.25">
       <c r="A14" s="18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>45</v>
@@ -35157,7 +35155,7 @@
         <v>68190.2</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M14" s="18">
         <v>-120</v>
@@ -35183,17 +35181,17 @@
     </row>
     <row r="15" spans="1:26" ht="14.25">
       <c r="A15" s="18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>45</v>
@@ -35214,7 +35212,7 @@
         <v>68190.2</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M15" s="18">
         <v>-120</v>
@@ -35240,17 +35238,17 @@
     </row>
     <row r="16" spans="1:26" ht="14.25">
       <c r="A16" s="18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>45</v>
@@ -35271,7 +35269,7 @@
         <v>68190.2</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M16" s="18">
         <v>-120</v>
@@ -35297,17 +35295,17 @@
     </row>
     <row r="17" spans="1:26" ht="14.25">
       <c r="A17" s="18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>45</v>
@@ -35328,7 +35326,7 @@
         <v>68190.2</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M17" s="18">
         <v>-120</v>
@@ -35354,17 +35352,17 @@
     </row>
     <row r="18" spans="1:26" ht="14.25">
       <c r="A18" s="18" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>45</v>
@@ -35385,7 +35383,7 @@
         <v>68190.2</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M18" s="18">
         <v>-120</v>
@@ -35411,17 +35409,17 @@
     </row>
     <row r="19" spans="1:26" ht="14.25">
       <c r="A19" s="18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>45</v>
@@ -35442,7 +35440,7 @@
         <v>68190.2</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M19" s="18">
         <v>-120</v>
@@ -35468,17 +35466,17 @@
     </row>
     <row r="20" spans="1:26" ht="14.25">
       <c r="A20" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F20" s="18" t="s">
         <v>45</v>
@@ -35499,7 +35497,7 @@
         <v>68190.2</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M20" s="18">
         <v>-120</v>
@@ -36264,7 +36262,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -36287,10 +36285,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -37297,15 +37295,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -38066,7 +38064,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25">
@@ -38089,10 +38087,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>

</xml_diff>

<commit_message>
Fixed "Assignment" and added tsv for "Fujita_2010_gsa"
</commit_message>
<xml_diff>
--- a/SBTAB_Fujita_2010.xlsx
+++ b/SBTAB_Fujita_2010.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santos\Documents\GitHub\Subcellular_workflow\Matlab\Model\Model_Fujita_2010\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE475DB8-DBED-4099-8C94-909CEAE8E957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71630B2D-71AF-4CAE-B0E2-F2A58B8B6D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="7500" tabRatio="857" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="857" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compartment" sheetId="71" r:id="rId1"/>
@@ -290,9 +290,6 @@
   </si>
   <si>
     <t>&gt;S0</t>
-  </si>
-  <si>
-    <t>!Assignement</t>
   </si>
   <si>
     <t>!Interpolation</t>
@@ -900,6 +897,9 @@
   <si>
     <t>nanomole/liter</t>
   </si>
+  <si>
+    <t>!Assignment</t>
+  </si>
 </sst>
 </file>
 
@@ -1458,7 +1458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B57E33C-33F4-499F-BA51-8CC344DB1D85}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1469,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1483,18 +1483,18 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D3" s="35">
         <v>1.0000000000000001E-15</v>
@@ -1528,15 +1528,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -2297,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -2320,10 +2320,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -3321,15 +3321,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -4090,7 +4090,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -4113,10 +4113,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -5114,15 +5114,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -5883,7 +5883,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -5906,10 +5906,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -6907,15 +6907,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -7676,7 +7676,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -7699,10 +7699,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -8700,15 +8700,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -9469,7 +9469,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -9492,10 +9492,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -10474,11 +10474,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AA62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10503,7 +10503,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
@@ -10532,10 +10532,10 @@
         <v>19</v>
       </c>
       <c r="F2" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" s="29" t="s">
         <v>72</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>73</v>
       </c>
       <c r="H2" s="26" t="s">
         <v>20</v>
@@ -10553,10 +10553,10 @@
         <v>22</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D3" s="9">
         <v>68190.2</v>
@@ -10577,10 +10577,10 @@
         <v>23</v>
       </c>
       <c r="I3" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>91</v>
       </c>
       <c r="O3" s="26"/>
     </row>
@@ -10589,10 +10589,10 @@
         <v>24</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D4" s="26">
         <v>0</v>
@@ -10613,10 +10613,10 @@
         <v>23</v>
       </c>
       <c r="I4" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>91</v>
       </c>
       <c r="O4" s="26"/>
     </row>
@@ -10625,10 +10625,10 @@
         <v>25</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D5" s="26">
         <v>0</v>
@@ -10649,10 +10649,10 @@
         <v>23</v>
       </c>
       <c r="I5" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>91</v>
       </c>
       <c r="O5" s="26"/>
     </row>
@@ -10661,10 +10661,10 @@
         <v>26</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D6" s="9">
         <v>4.3309E-2</v>
@@ -10685,10 +10685,10 @@
         <v>23</v>
       </c>
       <c r="I6" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="J6" s="26" t="s">
-        <v>91</v>
       </c>
       <c r="O6" s="26"/>
     </row>
@@ -10697,10 +10697,10 @@
         <v>27</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D7" s="26">
         <v>0</v>
@@ -10721,10 +10721,10 @@
         <v>23</v>
       </c>
       <c r="I7" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="J7" s="26" t="s">
-        <v>91</v>
       </c>
       <c r="K7" s="32"/>
       <c r="L7" s="32"/>
@@ -10746,13 +10746,13 @@
     </row>
     <row r="8" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D8" s="9">
         <v>3.5431699999999999</v>
@@ -10773,22 +10773,22 @@
         <v>23</v>
       </c>
       <c r="I8" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="J8" s="26" t="s">
-        <v>91</v>
       </c>
       <c r="O8" s="26"/>
     </row>
     <row r="9" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="30" t="s">
-        <v>84</v>
-      </c>
       <c r="C9" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D9" s="26">
         <v>0</v>
@@ -10809,22 +10809,22 @@
         <v>23</v>
       </c>
       <c r="I9" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="J9" s="26" t="s">
-        <v>91</v>
       </c>
       <c r="O9" s="26"/>
     </row>
     <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D10" s="26">
         <v>0</v>
@@ -10845,22 +10845,22 @@
         <v>23</v>
       </c>
       <c r="I10" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="J10" s="26" t="s">
-        <v>91</v>
       </c>
       <c r="O10" s="26"/>
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D11" s="26">
         <v>0</v>
@@ -10881,22 +10881,22 @@
         <v>23</v>
       </c>
       <c r="I11" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="J11" s="26" t="s">
-        <v>91</v>
       </c>
       <c r="O11" s="26"/>
     </row>
     <row r="12" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D12" s="26">
         <v>0</v>
@@ -10917,22 +10917,22 @@
         <v>23</v>
       </c>
       <c r="I12" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="J12" s="26" t="s">
-        <v>91</v>
       </c>
       <c r="O12" s="26"/>
     </row>
     <row r="13" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D13" s="9">
         <v>68190.2</v>
@@ -10953,10 +10953,10 @@
         <v>23</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O13" s="26"/>
     </row>
@@ -11638,15 +11638,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -12407,7 +12407,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -12430,10 +12430,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -13431,15 +13431,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -14200,7 +14200,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -14223,10 +14223,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -15224,15 +15224,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -15993,7 +15993,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -16016,10 +16016,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -17017,15 +17017,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -17786,7 +17786,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -17809,10 +17809,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -18810,15 +18810,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -19579,7 +19579,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -19602,10 +19602,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -20610,7 +20610,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="7"/>
@@ -20685,17 +20685,17 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="15" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -20726,17 +20726,17 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" s="15" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -20767,17 +20767,17 @@
         <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -20808,17 +20808,17 @@
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -20843,23 +20843,23 @@
     </row>
     <row r="7" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7" s="15" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -20884,23 +20884,23 @@
     </row>
     <row r="8" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D8" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -20925,23 +20925,23 @@
     </row>
     <row r="9" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -20966,23 +20966,23 @@
     </row>
     <row r="10" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D10" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -21007,23 +21007,23 @@
     </row>
     <row r="11" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D11" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -21048,23 +21048,23 @@
     </row>
     <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D12" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -21089,23 +21089,23 @@
     </row>
     <row r="13" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D13" s="16" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -21243,15 +21243,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -22012,7 +22012,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -22035,10 +22035,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -23036,15 +23036,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -23805,7 +23805,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -23828,10 +23828,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -24829,15 +24829,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -25598,7 +25598,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -25621,10 +25621,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -26622,15 +26622,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -27391,7 +27391,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -27414,10 +27414,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -28415,15 +28415,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -29184,7 +29184,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -29207,10 +29207,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -30215,7 +30215,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -30277,10 +30277,10 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E3" s="25">
         <f t="shared" ref="E3:E16" si="0">10^F3</f>
@@ -30290,10 +30290,10 @@
         <v>-2.1714586807558929</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="10"/>
@@ -30311,10 +30311,10 @@
         <v>64</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E4" s="25">
         <f t="shared" si="0"/>
@@ -30324,10 +30324,10 @@
         <v>-1.3898830445880721</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="10"/>
@@ -30345,10 +30345,10 @@
         <v>65</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E5" s="25">
         <f t="shared" si="0"/>
@@ -30358,10 +30358,10 @@
         <v>-4.8084651529932163</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="10"/>
@@ -30379,10 +30379,10 @@
         <v>66</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E6" s="25">
         <f t="shared" si="0"/>
@@ -30392,10 +30392,10 @@
         <v>-2.2861123053046994</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="10"/>
@@ -30413,10 +30413,10 @@
         <v>67</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E7" s="25">
         <f t="shared" si="0"/>
@@ -30426,10 +30426,10 @@
         <v>-1.5147272923617776</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="10"/>
@@ -30447,10 +30447,10 @@
         <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E8" s="25">
         <f t="shared" si="0"/>
@@ -30460,10 +30460,10 @@
         <v>-1.0012203432596507</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="10"/>
@@ -30481,10 +30481,10 @@
         <v>69</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E9" s="25">
         <f t="shared" si="0"/>
@@ -30494,10 +30494,10 @@
         <v>-5.6773900160161705</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="10"/>
@@ -30515,10 +30515,10 @@
         <v>70</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E10" s="25">
         <f t="shared" si="0"/>
@@ -30528,10 +30528,10 @@
         <v>-14.285720547548516</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="10"/>
@@ -30546,13 +30546,13 @@
     </row>
     <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E11" s="25">
         <f t="shared" si="0"/>
@@ -30562,10 +30562,10 @@
         <v>-2.9154308710048689</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="10"/>
@@ -30580,13 +30580,13 @@
     </row>
     <row r="12" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E12" s="25">
         <f t="shared" si="0"/>
@@ -30596,10 +30596,10 @@
         <v>-1.4841764738077223</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="10"/>
@@ -30614,13 +30614,13 @@
     </row>
     <row r="13" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E13" s="25">
         <f>10^F13</f>
@@ -30630,10 +30630,10 @@
         <v>-2.9465297153107599</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="10"/>
@@ -30648,13 +30648,13 @@
     </row>
     <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E14" s="25">
         <f t="shared" si="0"/>
@@ -30664,10 +30664,10 @@
         <v>-1.7158152480038114</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="10"/>
@@ -30682,13 +30682,13 @@
     </row>
     <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E15" s="25">
         <f t="shared" si="0"/>
@@ -30698,10 +30698,10 @@
         <v>-3.9731155198115515</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="10"/>
@@ -30716,13 +30716,13 @@
     </row>
     <row r="16" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E16" s="25">
         <f t="shared" si="0"/>
@@ -30732,10 +30732,10 @@
         <v>-3.9731155198115515</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="10"/>
@@ -30882,15 +30882,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -31651,7 +31651,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -31674,10 +31674,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -32675,15 +32675,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -33455,7 +33455,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
@@ -33546,10 +33546,10 @@
         <v>34</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D3" s="18" t="str">
         <f>_xlfn.CONCAT("SD_",A3)</f>
@@ -33559,7 +33559,7 @@
         <v>35</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>36</v>
@@ -33569,10 +33569,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L3" s="18"/>
       <c r="M3" s="16"/>
@@ -33601,10 +33601,10 @@
         <v>37</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D4" s="18" t="str">
         <f t="shared" ref="D4:D16" si="0">_xlfn.CONCAT("SD_",A4)</f>
@@ -33614,7 +33614,7 @@
         <v>35</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>36</v>
@@ -33624,10 +33624,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J4" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K4" s="17"/>
       <c r="L4" s="18"/>
@@ -33654,13 +33654,13 @@
     </row>
     <row r="5" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D5" s="18" t="str">
         <f t="shared" si="0"/>
@@ -33670,7 +33670,7 @@
         <v>35</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>36</v>
@@ -33680,10 +33680,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J5" s="34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K5" s="17"/>
       <c r="L5" s="18"/>
@@ -33710,10 +33710,10 @@
     </row>
     <row r="6" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D6" s="18" t="str">
         <f t="shared" si="0"/>
@@ -33723,7 +33723,7 @@
         <v>35</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>36</v>
@@ -33733,10 +33733,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
@@ -33763,10 +33763,10 @@
     </row>
     <row r="7" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D7" s="18" t="str">
         <f t="shared" si="0"/>
@@ -33776,7 +33776,7 @@
         <v>35</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>36</v>
@@ -33786,10 +33786,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
@@ -33816,10 +33816,10 @@
     </row>
     <row r="8" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D8" s="18" t="str">
         <f t="shared" si="0"/>
@@ -33829,7 +33829,7 @@
         <v>35</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>36</v>
@@ -33839,10 +33839,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
@@ -33869,10 +33869,10 @@
     </row>
     <row r="9" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="18" t="str">
@@ -33883,7 +33883,7 @@
         <v>35</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>36</v>
@@ -33893,10 +33893,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
@@ -33923,10 +33923,10 @@
     </row>
     <row r="10" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="18" t="str">
@@ -33937,7 +33937,7 @@
         <v>35</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>36</v>
@@ -33947,10 +33947,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
@@ -33977,10 +33977,10 @@
     </row>
     <row r="11" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="str">
@@ -33991,7 +33991,7 @@
         <v>35</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>36</v>
@@ -34001,10 +34001,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
@@ -34031,10 +34031,10 @@
     </row>
     <row r="12" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="18" t="str">
@@ -34045,7 +34045,7 @@
         <v>35</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>36</v>
@@ -34055,10 +34055,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
@@ -34085,10 +34085,10 @@
     </row>
     <row r="13" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="18" t="str">
@@ -34099,7 +34099,7 @@
         <v>35</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>36</v>
@@ -34109,10 +34109,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
@@ -34139,10 +34139,10 @@
     </row>
     <row r="14" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="18" t="str">
@@ -34153,7 +34153,7 @@
         <v>35</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G14" s="16" t="s">
         <v>36</v>
@@ -34163,10 +34163,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
@@ -34193,10 +34193,10 @@
     </row>
     <row r="15" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="18" t="str">
@@ -34207,7 +34207,7 @@
         <v>35</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>36</v>
@@ -34217,10 +34217,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
@@ -34247,10 +34247,10 @@
     </row>
     <row r="16" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>189</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>190</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="18" t="str">
@@ -34261,7 +34261,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G16" s="16" t="s">
         <v>36</v>
@@ -34271,10 +34271,10 @@
         <v>\ce{[Total_{\text{C}}]}</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J16" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
@@ -34410,7 +34410,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
@@ -34460,16 +34460,16 @@
         <v>71</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="I2" s="17" t="s">
-        <v>151</v>
-      </c>
       <c r="J2" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>21</v>
@@ -34507,7 +34507,7 @@
         <v>44</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>45</v>
@@ -34528,7 +34528,7 @@
         <v>68190.2</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M3" s="18">
         <v>-120</v>
@@ -34554,17 +34554,17 @@
     </row>
     <row r="4" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>74</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>75</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>45</v>
@@ -34585,7 +34585,7 @@
         <v>68190.2</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M4" s="18">
         <v>-120</v>
@@ -34611,17 +34611,17 @@
     </row>
     <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>77</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>45</v>
@@ -34642,7 +34642,7 @@
         <v>68190.2</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M5" s="18">
         <v>-120</v>
@@ -34668,17 +34668,17 @@
     </row>
     <row r="6" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>197</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>198</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>45</v>
@@ -34699,7 +34699,7 @@
         <v>68190.2</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M6" s="18">
         <v>-120</v>
@@ -34725,17 +34725,17 @@
     </row>
     <row r="7" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>200</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>201</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>45</v>
@@ -34756,7 +34756,7 @@
         <v>68190.2</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M7" s="18">
         <v>-120</v>
@@ -34782,17 +34782,17 @@
     </row>
     <row r="8" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>202</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>203</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F8" s="18" t="s">
         <v>45</v>
@@ -34813,7 +34813,7 @@
         <v>68190.2</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M8" s="18">
         <v>-120</v>
@@ -34839,17 +34839,17 @@
     </row>
     <row r="9" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>204</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>205</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>45</v>
@@ -34870,7 +34870,7 @@
         <v>68190.2</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M9" s="18">
         <v>-120</v>
@@ -34896,17 +34896,17 @@
     </row>
     <row r="10" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>206</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>207</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>45</v>
@@ -34927,7 +34927,7 @@
         <v>68190.2</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M10" s="18">
         <v>-120</v>
@@ -34953,17 +34953,17 @@
     </row>
     <row r="11" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>208</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>209</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>45</v>
@@ -34984,7 +34984,7 @@
         <v>68190.2</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M11" s="18">
         <v>-120</v>
@@ -35010,17 +35010,17 @@
     </row>
     <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>210</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>211</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>45</v>
@@ -35041,7 +35041,7 @@
         <v>68190.2</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M12" s="18">
         <v>-120</v>
@@ -35067,17 +35067,17 @@
     </row>
     <row r="13" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>212</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>213</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>45</v>
@@ -35098,7 +35098,7 @@
         <v>68190.2</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M13" s="18">
         <v>-120</v>
@@ -35124,17 +35124,17 @@
     </row>
     <row r="14" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>214</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>215</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>45</v>
@@ -35155,7 +35155,7 @@
         <v>68190.2</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M14" s="18">
         <v>-120</v>
@@ -35181,17 +35181,17 @@
     </row>
     <row r="15" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>216</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>217</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>45</v>
@@ -35212,7 +35212,7 @@
         <v>68190.2</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M15" s="18">
         <v>-120</v>
@@ -35238,17 +35238,17 @@
     </row>
     <row r="16" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>218</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>219</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>45</v>
@@ -35269,7 +35269,7 @@
         <v>68190.2</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M16" s="18">
         <v>-120</v>
@@ -35295,17 +35295,17 @@
     </row>
     <row r="17" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>220</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>221</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>45</v>
@@ -35326,7 +35326,7 @@
         <v>68190.2</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M17" s="18">
         <v>-120</v>
@@ -35352,17 +35352,17 @@
     </row>
     <row r="18" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>222</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>223</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>45</v>
@@ -35383,7 +35383,7 @@
         <v>68190.2</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M18" s="18">
         <v>-120</v>
@@ -35409,17 +35409,17 @@
     </row>
     <row r="19" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>224</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>225</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>45</v>
@@ -35440,7 +35440,7 @@
         <v>68190.2</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M19" s="18">
         <v>-120</v>
@@ -35466,17 +35466,17 @@
     </row>
     <row r="20" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>226</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>227</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18" t="s">
         <v>44</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F20" s="18" t="s">
         <v>45</v>
@@ -35497,7 +35497,7 @@
         <v>68190.2</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M20" s="18">
         <v>-120</v>
@@ -36262,7 +36262,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -36285,10 +36285,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -37295,15 +37295,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -38064,7 +38064,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
@@ -38087,10 +38087,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>

</xml_diff>